<commit_message>
transferred med4 noenz exports to data dir
</commit_message>
<xml_diff>
--- a/analyses/uwpr-apr2017/unipept-lca/233-peaks105-dno-nomods-lca.xlsx
+++ b/analyses/uwpr-apr2017/unipept-lca/233-peaks105-dno-nomods-lca.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/uwpr-apr2017/unipept-lca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92828B3A-8872-CD42-B0CA-08EB32FEE214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754891C2-324C-E643-8881-B36E60CE4C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="4060" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="1760" yWindow="2340" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="233-peaks105-dno-nomods-lca" sheetId="1" r:id="rId1"/>
+    <sheet name="all fungi" sheetId="2" r:id="rId2"/>
+    <sheet name="all cyanos" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'233-peaks105-dno-nomods-lca'!$A$1:$AH$1130</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7257" uniqueCount="5141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7601" uniqueCount="5141">
   <si>
     <t>peptide</t>
   </si>
@@ -15448,7 +15453,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -16282,10 +16287,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -40321,6 +40328,1122 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AH1130" xr:uid="{1B13DCA4-DE42-5945-A910-54C780226007}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68532412-1BDD-2648-9E70-BC1622C1DE2E}">
+  <dimension ref="A1:AH23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H3" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" t="s">
+        <v>256</v>
+      </c>
+      <c r="N3" t="s">
+        <v>257</v>
+      </c>
+      <c r="S3" t="s">
+        <v>258</v>
+      </c>
+      <c r="W3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B5" t="s">
+        <v>633</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
+        <v>634</v>
+      </c>
+      <c r="K5" t="s">
+        <v>635</v>
+      </c>
+      <c r="N5" t="s">
+        <v>636</v>
+      </c>
+      <c r="S5" t="s">
+        <v>637</v>
+      </c>
+      <c r="W5" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>695</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>985</v>
+      </c>
+      <c r="B7" t="s">
+        <v>986</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
+        <v>987</v>
+      </c>
+      <c r="K7" t="s">
+        <v>988</v>
+      </c>
+      <c r="N7" t="s">
+        <v>989</v>
+      </c>
+      <c r="S7" t="s">
+        <v>986</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>990</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1082</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1083</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1085</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1136</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>1137</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1432</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1433</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1434</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1435</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1436</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>634</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1626</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1627</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1628</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="W11" t="s">
+        <v>1630</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2009</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" t="s">
+        <v>2011</v>
+      </c>
+      <c r="S12" t="s">
+        <v>2012</v>
+      </c>
+      <c r="W12" t="s">
+        <v>2013</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>2010</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>594</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2374</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" t="s">
+        <v>987</v>
+      </c>
+      <c r="K13" t="s">
+        <v>2376</v>
+      </c>
+      <c r="N13" t="s">
+        <v>2377</v>
+      </c>
+      <c r="S13" t="s">
+        <v>2378</v>
+      </c>
+      <c r="W13" t="s">
+        <v>2379</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>2375</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>2380</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>2381</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>2382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" t="s">
+        <v>2644</v>
+      </c>
+      <c r="N14" t="s">
+        <v>2643</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>2645</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2896</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>2897</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>2898</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>2899</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2945</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2946</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" t="s">
+        <v>63</v>
+      </c>
+      <c r="N16" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16" t="s">
+        <v>56</v>
+      </c>
+      <c r="W16" t="s">
+        <v>2947</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>2946</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3544</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3545</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>987</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2376</v>
+      </c>
+      <c r="N17" t="s">
+        <v>2377</v>
+      </c>
+      <c r="W17" t="s">
+        <v>3545</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3802</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3803</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3804</v>
+      </c>
+      <c r="S18" t="s">
+        <v>3805</v>
+      </c>
+      <c r="W18" t="s">
+        <v>3803</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>1592</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>2519</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4318</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4319</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>987</v>
+      </c>
+      <c r="K19" t="s">
+        <v>2376</v>
+      </c>
+      <c r="N19" t="s">
+        <v>4320</v>
+      </c>
+      <c r="S19" t="s">
+        <v>4321</v>
+      </c>
+      <c r="W19" t="s">
+        <v>4322</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>4319</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>1592</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>4323</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>4324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4357</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4358</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>254</v>
+      </c>
+      <c r="H20" t="s">
+        <v>255</v>
+      </c>
+      <c r="J20" t="s">
+        <v>256</v>
+      </c>
+      <c r="N20" t="s">
+        <v>4359</v>
+      </c>
+      <c r="S20" t="s">
+        <v>4360</v>
+      </c>
+      <c r="W20" t="s">
+        <v>4361</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>4358</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>2519</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>4362</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4373</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>4374</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4840</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>924</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>4841</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>4842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4845</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4846</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4847</v>
+      </c>
+      <c r="J23" t="s">
+        <v>4848</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4849</v>
+      </c>
+      <c r="S23" t="s">
+        <v>4850</v>
+      </c>
+      <c r="W23" t="s">
+        <v>4851</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>4846</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965F6074-8116-1544-ADF3-33611F6F2EF6}">
+  <dimension ref="A1:AH3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3121</v>
+      </c>
+      <c r="S3" t="s">
+        <v>3122</v>
+      </c>
+      <c r="W3" t="s">
+        <v>3120</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>